<commit_message>
Login and ApplicationForm page completed successfully
</commit_message>
<xml_diff>
--- a/src/Data/UserDetail.xlsx
+++ b/src/Data/UserDetail.xlsx
@@ -14,24 +14,78 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Account No</t>
+  </si>
+  <si>
+    <t>Mobile No</t>
+  </si>
+  <si>
+    <t>Email Address</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Account Type</t>
+  </si>
+  <si>
+    <t>Account Balance</t>
+  </si>
+  <si>
+    <t>Last Deposite</t>
+  </si>
+  <si>
+    <t>Last Transaction</t>
+  </si>
+  <si>
+    <t>Last Transaction Date/Time</t>
+  </si>
   <si>
     <t>Shubhash Singh</t>
   </si>
   <si>
+    <t>17077480451758864</t>
+  </si>
+  <si>
+    <t>9381560406</t>
+  </si>
+  <si>
+    <t>subhashsingh2059@gmail.com</t>
+  </si>
+  <si>
     <t>Zapkto9@</t>
   </si>
   <si>
-    <t>9381560406</t>
-  </si>
-  <si>
-    <t>subhashsingh2059@gmail.com</t>
+    <t>Current</t>
+  </si>
+  <si>
+    <t>1500</t>
+  </si>
+  <si>
+    <t>Nisha Pandey</t>
+  </si>
+  <si>
+    <t>17077481098644571</t>
+  </si>
+  <si>
+    <t>7337498907</t>
+  </si>
+  <si>
+    <t>neshapandey4@gmail.com</t>
+  </si>
+  <si>
+    <t>Nisha</t>
   </si>
   <si>
     <t>Saving</t>
   </si>
   <si>
-    <t>15000</t>
+    <t>2500</t>
   </si>
 </sst>
 </file>
@@ -378,21 +432,22 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="25.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="21.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="14.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="37.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="2" width="20.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="2" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="2" width="22.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="2" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="2" width="26.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="25.14785714285714"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="21.719285714285714"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="14.43357142857143"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="37.57642857142857"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="20.14785714285714"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="17.862142857142857"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="22.862142857142857"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="13.005"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="20.719285714285714"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="26.290714285714284"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
@@ -405,6 +460,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
       <c r="A2" s="1"/>
@@ -416,44 +472,59 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+    <row r="3">
+      <c r="A3" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s" s="2">
+        <v>16</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" s="1"/>
+    <row r="4">
+      <c r="A4" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s" s="2">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s" s="2">
+        <v>23</v>
+      </c>
+      <c r="H4" t="s" s="2">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
TransactionSection is being modified
</commit_message>
<xml_diff>
--- a/src/Data/UserDetail.xlsx
+++ b/src/Data/UserDetail.xlsx
@@ -14,15 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Account No</t>
-  </si>
-  <si>
-    <t>Mobile No</t>
+    <t>Account Number</t>
+  </si>
+  <si>
+    <t>Phine Number</t>
   </si>
   <si>
     <t>Email Address</t>
@@ -34,7 +34,7 @@
     <t>Account Type</t>
   </si>
   <si>
-    <t>Account Balance</t>
+    <t>Balance</t>
   </si>
   <si>
     <t>Last Deposite</t>
@@ -43,7 +43,7 @@
     <t>Last Transaction</t>
   </si>
   <si>
-    <t>Last Transaction Date/Time</t>
+    <t>Last Trans Details</t>
   </si>
   <si>
     <t>Shubhash Singh</t>
@@ -67,6 +67,9 @@
     <t>1500</t>
   </si>
   <si>
+    <t>+ 1500</t>
+  </si>
+  <si>
     <t>Nisha Pandey</t>
   </si>
   <si>
@@ -86,6 +89,9 @@
   </si>
   <si>
     <t>2500</t>
+  </si>
+  <si>
+    <t>+ 2500</t>
   </si>
 </sst>
 </file>
@@ -438,16 +444,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="25.14785714285714"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="21.719285714285714"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="14.43357142857143"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="37.57642857142857"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="20.14785714285714"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="17.862142857142857"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="22.862142857142857"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="13.005"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="20.719285714285714"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="26.290714285714284"/>
+    <col min="1" max="1" style="2" width="25.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="21.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="2" width="14.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="2" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="2" width="20.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="2" width="17.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="2" width="22.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="2" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="2" width="20.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="2" width="26.290714285714284" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
@@ -463,68 +469,96 @@
       <c r="J1" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s" s="2">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s" s="2">
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s" s="2">
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s" s="2">
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s" s="2">
+      <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F3" t="s" s="2">
+      <c r="F3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G3" t="s" s="2">
+      <c r="G3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H3" t="s" s="2">
+      <c r="H3" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="I3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="1"/>
     </row>
-    <row r="4">
-      <c r="A4" t="s" s="2">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s" s="2">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
+      <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s" s="2">
+      <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D4" t="s" s="2">
+      <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E4" t="s" s="2">
+      <c r="D4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F4" t="s" s="2">
+      <c r="E4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G4" t="s" s="2">
+      <c r="F4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H4" t="s" s="2">
-        <v>23</v>
-      </c>
+      <c r="G4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Some last effort are still required
</commit_message>
<xml_diff>
--- a/src/Data/UserDetail.xlsx
+++ b/src/Data/UserDetail.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -22,10 +22,10 @@
     <t>Account Number</t>
   </si>
   <si>
-    <t>Phine Number</t>
-  </si>
-  <si>
-    <t>Email Address</t>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>Email</t>
   </si>
   <si>
     <t>Password</t>
@@ -43,16 +43,19 @@
     <t>Last Transaction</t>
   </si>
   <si>
-    <t>Last Trans Details</t>
+    <t>Transaction Time</t>
+  </si>
+  <si>
+    <t>Transaction Details</t>
   </si>
   <si>
     <t>Shubhash Singh</t>
   </si>
   <si>
-    <t>17077480451758864</t>
-  </si>
-  <si>
-    <t>9381560406</t>
+    <t>17078798351431456</t>
+  </si>
+  <si>
+    <t>+91-9381560406</t>
   </si>
   <si>
     <t>subhashsingh2059@gmail.com</t>
@@ -61,37 +64,19 @@
     <t>Zapkto9@</t>
   </si>
   <si>
-    <t>Current</t>
-  </si>
-  <si>
-    <t>1500</t>
-  </si>
-  <si>
-    <t>+ 1500</t>
-  </si>
-  <si>
-    <t>Nisha Pandey</t>
-  </si>
-  <si>
-    <t>17077481098644571</t>
-  </si>
-  <si>
-    <t>7337498907</t>
-  </si>
-  <si>
-    <t>neshapandey4@gmail.com</t>
-  </si>
-  <si>
-    <t>Nisha</t>
-  </si>
-  <si>
     <t>Saving</t>
   </si>
   <si>
-    <t>2500</t>
-  </si>
-  <si>
-    <t>+ 2500</t>
+    <t>15000</t>
+  </si>
+  <si>
+    <t>+ 15000</t>
+  </si>
+  <si>
+    <t>2024-02-14 at 08:33:56</t>
+  </si>
+  <si>
+    <t>+15000 Initial Deposite on</t>
   </si>
 </sst>
 </file>
@@ -161,28 +146,28 @@
         <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F818D"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="0000FF"/>
@@ -438,127 +423,94 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="25.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="21.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="14.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="37.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="2" width="20.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="2" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="2" width="22.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="2" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="2" width="20.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="2" width="26.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="13.005"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="25.005"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="26.290714285714284"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="33.43357142857143"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="13.005"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="13.005"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="13.005"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="23.862142857142857"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="26.290714285714284"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="25.14785714285714"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="44.29071428571429"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row r="2">
+      <c r="A2" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="B2" t="s" s="2">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="C2" t="s" s="2">
         <v>13</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="D2" t="s" s="2">
         <v>14</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="E2" t="s" s="2">
         <v>15</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="F2" t="s" s="2">
         <v>16</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="G2" t="s" s="2">
         <v>17</v>
       </c>
-      <c r="J3" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
-      <c r="A4" s="1" t="s">
+      <c r="H2" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s" s="2">
         <v>18</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="J2" t="s" s="2">
         <v>19</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="K2" t="s" s="2">
         <v>20</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
LoginPage AccountDetail and ApplicationForm are fully completed
</commit_message>
<xml_diff>
--- a/src/Data/UserDetail.xlsx
+++ b/src/Data/UserDetail.xlsx
@@ -429,17 +429,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="13.005"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="25.005"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="26.290714285714284"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="33.43357142857143"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="13.005"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="13.005"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="13.005"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="23.862142857142857"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="26.290714285714284"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="25.14785714285714"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="44.29071428571429"/>
+    <col min="1" max="1" style="2" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="25.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="2" width="26.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="2" width="33.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="2" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="2" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="2" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="2" width="23.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="2" width="26.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="2" width="25.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="2" width="44.29071428571429" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
@@ -477,38 +477,38 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s" s="2">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
+      <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s" s="2">
+      <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s" s="2">
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s" s="2">
+      <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s" s="2">
+      <c r="E2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s" s="2">
+      <c r="F2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G2" t="s" s="2">
+      <c r="G2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H2" t="s" s="2">
+      <c r="H2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I2" t="s" s="2">
+      <c r="I2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J2" t="s" s="2">
+      <c r="J2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K2" t="s" s="2">
+      <c r="K2" s="1" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
All files final form updated
</commit_message>
<xml_diff>
--- a/src/Data/UserDetail.xlsx
+++ b/src/Data/UserDetail.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -125,6 +125,60 @@
   </si>
   <si>
     <t>Sent 1000 to Nisha Pandey</t>
+  </si>
+  <si>
+    <t>26000.0</t>
+  </si>
+  <si>
+    <t>1000.0</t>
+  </si>
+  <si>
+    <t>+10000</t>
+  </si>
+  <si>
+    <t>-10000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> on 2024-02-16 at 16:46:59</t>
+  </si>
+  <si>
+    <t>Received 10000 from Shubhash Singh</t>
+  </si>
+  <si>
+    <t>Sent 10000 to Nisha Pandey</t>
+  </si>
+  <si>
+    <t>17080824033178231</t>
+  </si>
+  <si>
+    <t>+91-9381560406</t>
+  </si>
+  <si>
+    <t>subhashsingh2059@gmail.com</t>
+  </si>
+  <si>
+    <t>120000</t>
+  </si>
+  <si>
+    <t>+ 120000</t>
+  </si>
+  <si>
+    <t>2024-02-16 at 16:50:04</t>
+  </si>
+  <si>
+    <t>+120000 Initial Deposite on</t>
+  </si>
+  <si>
+    <t>11000</t>
+  </si>
+  <si>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>2024-02-16 at 19:50:01</t>
+  </si>
+  <si>
+    <t>+10000 Deposite on</t>
   </si>
 </sst>
 </file>
@@ -1108,7 +1162,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
@@ -1183,19 +1237,19 @@
         <v>16</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" ht="18" customHeight="1" spans="1:11">
@@ -1218,19 +1272,54 @@
         <v>16</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>36</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="1">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s" s="1">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s" s="1">
+        <v>45</v>
+      </c>
+      <c r="D4" t="s" s="1">
+        <v>46</v>
+      </c>
+      <c r="E4" t="s" s="1">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s" s="1">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="H4" t="s" s="1">
+        <v>47</v>
+      </c>
+      <c r="I4" t="s" s="1">
+        <v>48</v>
+      </c>
+      <c r="J4" t="s" s="1">
+        <v>49</v>
+      </c>
+      <c r="K4" t="s" s="1">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>